<commit_message>
modified excel for flask task
</commit_message>
<xml_diff>
--- a/students_flask/python_students.xlsx
+++ b/students_flask/python_students.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\projects\codify-python3-2023\students_flask\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65633EFE-0445-4804-A48E-3FBCD93ABE43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2ED70A5-7F18-45A1-8608-1D37984095A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -354,262 +354,412 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A50"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>61.285714285714299</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>60.642857142857103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>59.357142857142897</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>58.714285714285701</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>58.071428571428598</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>57.428571428571402</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>56.785714285714299</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>56.142857142857103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>55.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>54.857142857142897</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>54.214285714285701</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>53.571428571428598</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>52.928571428571402</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>52.285714285714299</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>51.642857142857103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>50.357142857142897</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>49.714285714285701</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>49.071428571428598</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>48.428571428571402</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>47.785714285714299</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>47.142857142857103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>46.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>45.857142857142897</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>45.214285714285701</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>44.571428571428598</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>43.928571428571402</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>43.285714285714299</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <v>42.642857142857103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B39">
+        <v>41.357142857142897</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <v>40.714285714285701</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>40.071428571428598</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <v>39.428571428571402</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <v>38.785714285714299</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <v>38.142857142857103</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B45">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B46">
+        <v>36.857142857142897</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B47">
+        <v>36.214285714285701</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B48">
+        <v>35.571428571428598</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B49">
+        <v>34.928571428571402</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>1</v>
+      </c>
+      <c r="B50">
+        <v>34.285714285714299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified excel for hw2
</commit_message>
<xml_diff>
--- a/students_flask/python_students.xlsx
+++ b/students_flask/python_students.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\projects\codify-python3-2023\students_flask\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2ED70A5-7F18-45A1-8608-1D37984095A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB238322-FFBB-4399-8EF9-882E45CD2199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -354,412 +354,562 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>83</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <v>42</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="B5">
         <v>86</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
       <c r="B6">
         <v>44</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7">
         <v>73</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>76.6666666666667</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8">
         <v>61.285714285714299</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>77.095238095238102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>0</v>
       </c>
       <c r="B9">
         <v>60.642857142857103</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>77.523809523809504</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1</v>
       </c>
       <c r="B10">
         <v>60</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>77.952380952381006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>2</v>
       </c>
       <c r="B11">
         <v>59.357142857142897</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>78.380952380952394</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>3</v>
       </c>
       <c r="B12">
         <v>58.714285714285701</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>78.809523809523796</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>0</v>
       </c>
       <c r="B13">
         <v>58.071428571428598</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>79.238095238095298</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>1</v>
       </c>
       <c r="B14">
         <v>57.428571428571402</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>79.6666666666667</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>2</v>
       </c>
       <c r="B15">
         <v>56.785714285714299</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <v>80.095238095238102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
       <c r="B16">
         <v>56.142857142857103</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>80.523809523809504</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>0</v>
       </c>
       <c r="B17">
         <v>55.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>80.952380952381006</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>1</v>
       </c>
       <c r="B18">
         <v>54.857142857142897</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>81.380952380952394</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>2</v>
       </c>
       <c r="B19">
         <v>54.214285714285701</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <v>81.809523809523796</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>3</v>
       </c>
       <c r="B20">
         <v>53.571428571428598</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>82.238095238095298</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>0</v>
       </c>
       <c r="B21">
         <v>52.928571428571402</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <v>82.6666666666667</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>1</v>
       </c>
       <c r="B22">
         <v>52.285714285714299</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <v>83.095238095238102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>2</v>
       </c>
       <c r="B23">
         <v>51.642857142857103</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <v>83.523809523809504</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>3</v>
       </c>
       <c r="B24">
         <v>51</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <v>83.952380952381006</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>0</v>
       </c>
       <c r="B25">
         <v>50.357142857142897</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <v>84.380952380952394</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>1</v>
       </c>
       <c r="B26">
         <v>49.714285714285701</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26">
+        <v>84.809523809523796</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>2</v>
       </c>
       <c r="B27">
         <v>49.071428571428598</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <v>85.238095238095298</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>3</v>
       </c>
       <c r="B28">
         <v>48.428571428571402</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <v>85.6666666666667</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>0</v>
       </c>
       <c r="B29">
         <v>47.785714285714299</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <v>86.095238095238102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>1</v>
       </c>
       <c r="B30">
         <v>47.142857142857103</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <v>86.523809523809504</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>2</v>
       </c>
       <c r="B31">
         <v>46.5</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <v>86.952380952381006</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>3</v>
       </c>
       <c r="B32">
         <v>45.857142857142897</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32">
+        <v>87.380952380952394</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>0</v>
       </c>
       <c r="B33">
         <v>45.214285714285701</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <v>87.809523809523796</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>1</v>
       </c>
       <c r="B34">
         <v>44.571428571428598</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34">
+        <v>88.238095238095298</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>2</v>
       </c>
       <c r="B35">
         <v>43.928571428571402</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C35">
+        <v>88.6666666666667</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>3</v>
       </c>
       <c r="B36">
         <v>43.285714285714299</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C36">
+        <v>89.095238095238102</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>0</v>
       </c>
       <c r="B37">
         <v>42.642857142857103</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C37">
+        <v>89.523809523809604</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>1</v>
       </c>
       <c r="B38">
         <v>42</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C38">
+        <v>89.952380952381006</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>2</v>
       </c>
       <c r="B39">
         <v>41.357142857142897</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C39">
+        <v>90.380952380952394</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>3</v>
       </c>
       <c r="B40">
         <v>40.714285714285701</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C40">
+        <v>90.809523809523796</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>0</v>
       </c>
       <c r="B41">
         <v>40.071428571428598</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C41">
+        <v>91.238095238095298</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>1</v>
       </c>
       <c r="B42">
         <v>39.428571428571402</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C42">
+        <v>91.6666666666667</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>2</v>
       </c>
       <c r="B43">
         <v>38.785714285714299</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C43">
+        <v>92.095238095238102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>3</v>
       </c>
       <c r="B44">
         <v>38.142857142857103</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C44">
+        <v>92.523809523809604</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>0</v>
       </c>
       <c r="B45">
         <v>37.5</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C45">
+        <v>92.952380952381006</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>1</v>
       </c>
       <c r="B46">
         <v>36.857142857142897</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C46">
+        <v>93.380952380952394</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>2</v>
       </c>
       <c r="B47">
         <v>36.214285714285701</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C47">
+        <v>93.809523809523796</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>3</v>
       </c>
       <c r="B48">
         <v>35.571428571428598</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C48">
+        <v>94.238095238095298</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>0</v>
       </c>
       <c r="B49">
         <v>34.928571428571402</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C49">
+        <v>94.6666666666667</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>1</v>
       </c>
       <c r="B50">
         <v>34.285714285714299</v>
+      </c>
+      <c r="C50">
+        <v>95.095238095238102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hw flask change row
</commit_message>
<xml_diff>
--- a/students_flask/python_students.xlsx
+++ b/students_flask/python_students.xlsx
@@ -440,14 +440,18 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Kaium</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>42</v>
-      </c>
-      <c r="C4" t="n">
-        <v>43</v>
+          <t>Тимур</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
       </c>
     </row>
     <row r="5">

</xml_diff>